<commit_message>
uplift ratelimit based bb tests
</commit_message>
<xml_diff>
--- a/test/blackbox/testfiles/test_leave.xlsx
+++ b/test/blackbox/testfiles/test_leave.xlsx
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Annual Leave</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD</t>
+    <t xml:space="preserve">Kasna</t>
   </si>
   <si>
     <t xml:space="preserve">Leave request 28/03/2020</t>
@@ -211,10 +211,10 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="11.42"/>
   </cols>

</xml_diff>